<commit_message>
Roadmap update, Sw functions update
</commit_message>
<xml_diff>
--- a/Project checklist/Roadmap.xlsx
+++ b/Project checklist/Roadmap.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\2025\Projects\Home Temp Monitor\Project checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4F019B-78AB-4D74-B987-F2B32A54436D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F7ADDD-D969-483D-A166-4A589AEB393C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Home Temp Monitor Roadmap</t>
   </si>
@@ -39,9 +48,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>01.07.2025</t>
-  </si>
-  <si>
     <t>Project module:</t>
   </si>
   <si>
@@ -64,13 +70,46 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>- transform all repeatable code into functions</t>
+  </si>
+  <si>
+    <t>- create repetitive measurements that are added to the SD card</t>
+  </si>
+  <si>
+    <t>- create error log csv file</t>
+  </si>
+  <si>
+    <t>- create a base of errors that can occur</t>
+  </si>
+  <si>
+    <t>- make voltage monitor for supply (dummy)</t>
+  </si>
+  <si>
+    <t>- create debounce function?</t>
+  </si>
+  <si>
+    <t>- implement new buttons for menu/error handling</t>
+  </si>
+  <si>
+    <t>25.06.2025</t>
+  </si>
+  <si>
+    <t>- hightlight if humidity too high/low</t>
+  </si>
+  <si>
+    <t>To do list:</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,8 +141,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +168,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF269E3D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -129,18 +190,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -149,6 +225,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF269E3D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -423,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AD9"/>
+  <dimension ref="A2:AD22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,81 +516,81 @@
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="10" customWidth="1"/>
     <col min="10" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="12" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
     </row>
     <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -521,69 +602,408 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="3"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>9</v>
+      <c r="I8" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" t="s">
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I9" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+    </row>
+    <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
+    </row>
+    <row r="14" spans="1:30" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="23">
+    <mergeCell ref="N18:AB18"/>
+    <mergeCell ref="N19:AB19"/>
+    <mergeCell ref="N20:AB20"/>
+    <mergeCell ref="N21:AB21"/>
+    <mergeCell ref="N22:AB22"/>
+    <mergeCell ref="B18:K18"/>
+    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="B20:K20"/>
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="B22:K22"/>
+    <mergeCell ref="A12:AD13"/>
+    <mergeCell ref="B15:K15"/>
+    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B17:K17"/>
+    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="N15:AB15"/>
+    <mergeCell ref="N16:AB16"/>
+    <mergeCell ref="N17:AB17"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="A2:AD3"/>
     <mergeCell ref="B7:C8"/>

</xml_diff>